<commit_message>
dynamatic change drop down box
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -6331,17 +6331,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="10.9" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.25" style="6" customWidth="1"/>
-    <col min="2" max="2" width="6.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.625" style="6" customWidth="1"/>
     <col min="6" max="6" width="41.5" style="3" customWidth="1"/>
     <col min="7" max="16384" width="11.25" style="1"/>
   </cols>

</xml_diff>